<commit_message>
still fixing maintenance function
</commit_message>
<xml_diff>
--- a/shipClassTests/testResults/Ship_w_Parallel_Sys.xlsx
+++ b/shipClassTests/testResults/Ship_w_Parallel_Sys.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="28">
   <si>
     <t>Time Step</t>
   </si>
@@ -505,7 +505,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -596,7 +596,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -611,7 +611,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -635,7 +635,7 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -650,7 +650,7 @@
         <v>1</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -674,7 +674,7 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -689,7 +689,7 @@
         <v>1</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -713,7 +713,7 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -728,7 +728,7 @@
         <v>1</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -752,7 +752,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -767,7 +767,7 @@
         <v>1</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -791,7 +791,7 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -806,7 +806,7 @@
         <v>1</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -830,7 +830,7 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -845,7 +845,7 @@
         <v>1</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -869,7 +869,7 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -884,7 +884,7 @@
         <v>1</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -908,7 +908,7 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -923,7 +923,7 @@
         <v>1</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -947,7 +947,7 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -962,7 +962,7 @@
         <v>1</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12">
         <v>1</v>
@@ -983,13 +983,13 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -1001,7 +1001,7 @@
         <v>1</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -1017,48 +1017,204 @@
         <v>0</v>
       </c>
     </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="3">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14" s="4">
+        <v>1</v>
+      </c>
+      <c r="L14" s="3">
+        <f>IF(B14 = G14, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="3">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15" s="4">
+        <v>1</v>
+      </c>
+      <c r="L15" s="3">
+        <f>IF(B15 = G15, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="3">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16" s="4">
+        <v>1</v>
+      </c>
+      <c r="L16" s="3">
+        <f>IF(B16 = G16, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="3">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17" s="4">
+        <v>1</v>
+      </c>
+      <c r="L17" s="3">
+        <f>IF(B17 = G17, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C14">
+  <conditionalFormatting sqref="C2:C18">
     <cfRule type="notContainsBlanks" dxfId="0" priority="2">
       <formula>LEN(TRIM(C2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D14">
+  <conditionalFormatting sqref="D2:D18">
     <cfRule type="notContainsBlanks" dxfId="0" priority="3">
       <formula>LEN(TRIM(D2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E14">
+  <conditionalFormatting sqref="E2:E18">
     <cfRule type="notContainsBlanks" dxfId="1" priority="4">
       <formula>LEN(TRIM(E2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F14">
+  <conditionalFormatting sqref="F2:F18">
     <cfRule type="notContainsBlanks" dxfId="1" priority="5">
       <formula>LEN(TRIM(F2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H14">
+  <conditionalFormatting sqref="H2:H18">
     <cfRule type="notContainsBlanks" dxfId="0" priority="6">
       <formula>LEN(TRIM(H2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I14">
+  <conditionalFormatting sqref="I2:I18">
     <cfRule type="notContainsBlanks" dxfId="0" priority="7">
       <formula>LEN(TRIM(I2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J14">
+  <conditionalFormatting sqref="J2:J18">
     <cfRule type="notContainsBlanks" dxfId="1" priority="8">
       <formula>LEN(TRIM(J2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K14">
+  <conditionalFormatting sqref="K2:K18">
     <cfRule type="notContainsBlanks" dxfId="1" priority="9">
       <formula>LEN(TRIM(K2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L13">
+  <conditionalFormatting sqref="L2:L17">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -1074,7 +1230,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R13"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1204,7 +1360,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1222,13 +1378,13 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" s="4">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3">
         <v>1</v>
@@ -1246,7 +1402,7 @@
         <v>1</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q3" s="4">
         <v>1</v>
@@ -1261,7 +1417,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1279,13 +1435,13 @@
         <v>1</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="4">
         <v>1</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -1303,7 +1459,7 @@
         <v>1</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q4" s="4">
         <v>1</v>
@@ -1318,7 +1474,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1336,13 +1492,13 @@
         <v>1</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="4">
         <v>1</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5">
         <v>1</v>
@@ -1360,7 +1516,7 @@
         <v>1</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q5" s="4">
         <v>1</v>
@@ -1375,7 +1531,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1393,13 +1549,13 @@
         <v>1</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="4">
         <v>1</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6">
         <v>1</v>
@@ -1417,7 +1573,7 @@
         <v>1</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q6" s="4">
         <v>1</v>
@@ -1432,10 +1588,10 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1450,13 +1606,13 @@
         <v>1</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="4">
         <v>1</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7">
         <v>1</v>
@@ -1474,7 +1630,7 @@
         <v>1</v>
       </c>
       <c r="P7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q7" s="4">
         <v>1</v>
@@ -1489,7 +1645,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1507,13 +1663,13 @@
         <v>1</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="4">
         <v>1</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8">
         <v>1</v>
@@ -1531,7 +1687,7 @@
         <v>1</v>
       </c>
       <c r="P8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q8" s="4">
         <v>1</v>
@@ -1546,7 +1702,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1564,13 +1720,13 @@
         <v>1</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="4">
         <v>1</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9">
         <v>1</v>
@@ -1588,7 +1744,7 @@
         <v>1</v>
       </c>
       <c r="P9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q9" s="4">
         <v>1</v>
@@ -1603,7 +1759,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1621,13 +1777,13 @@
         <v>1</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="4">
         <v>1</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10">
         <v>1</v>
@@ -1645,7 +1801,7 @@
         <v>1</v>
       </c>
       <c r="P10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q10" s="4">
         <v>1</v>
@@ -1660,7 +1816,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1678,13 +1834,13 @@
         <v>1</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="4">
         <v>1</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11">
         <v>1</v>
@@ -1702,7 +1858,7 @@
         <v>1</v>
       </c>
       <c r="P11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q11" s="4">
         <v>1</v>
@@ -1717,7 +1873,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1735,13 +1891,13 @@
         <v>1</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="4">
         <v>1</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12">
         <v>1</v>
@@ -1759,7 +1915,7 @@
         <v>1</v>
       </c>
       <c r="P12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q12" s="4">
         <v>1</v>
@@ -1774,7 +1930,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1792,13 +1948,13 @@
         <v>1</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" s="4">
         <v>1</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13">
         <v>1</v>
@@ -1816,7 +1972,7 @@
         <v>1</v>
       </c>
       <c r="P13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q13" s="4">
         <v>1</v>
@@ -1826,58 +1982,286 @@
         <v>0</v>
       </c>
     </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="3">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14" s="4">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>1</v>
+      </c>
+      <c r="R14" s="3">
+        <f>IF(B14 = J14, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="3">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15" s="4">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>1</v>
+      </c>
+      <c r="R15" s="3">
+        <f>IF(B15 = J15, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" s="3">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16" s="4">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>1</v>
+      </c>
+      <c r="R16" s="3">
+        <f>IF(B16 = J16, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" s="3">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17" s="4">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="4">
+        <v>1</v>
+      </c>
+      <c r="R17" s="3">
+        <f>IF(B17 = J17, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C14">
+  <conditionalFormatting sqref="C2:C18">
     <cfRule type="notContainsBlanks" dxfId="0" priority="2">
       <formula>LEN(TRIM(C2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D14">
+  <conditionalFormatting sqref="D2:D18">
     <cfRule type="notContainsBlanks" dxfId="0" priority="3">
       <formula>LEN(TRIM(D2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E14">
+  <conditionalFormatting sqref="E2:E18">
     <cfRule type="notContainsBlanks" dxfId="0" priority="4">
       <formula>LEN(TRIM(E2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F14">
+  <conditionalFormatting sqref="F2:F18">
     <cfRule type="notContainsBlanks" dxfId="1" priority="5">
       <formula>LEN(TRIM(F2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G14">
+  <conditionalFormatting sqref="G2:G18">
     <cfRule type="notContainsBlanks" dxfId="1" priority="6">
       <formula>LEN(TRIM(G2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K14">
+  <conditionalFormatting sqref="K2:K18">
     <cfRule type="notContainsBlanks" dxfId="0" priority="7">
       <formula>LEN(TRIM(K2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L14">
+  <conditionalFormatting sqref="L2:L18">
     <cfRule type="notContainsBlanks" dxfId="0" priority="8">
       <formula>LEN(TRIM(L2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M14">
+  <conditionalFormatting sqref="M2:M18">
     <cfRule type="notContainsBlanks" dxfId="0" priority="9">
       <formula>LEN(TRIM(M2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N14">
+  <conditionalFormatting sqref="N2:N18">
     <cfRule type="notContainsBlanks" dxfId="1" priority="10">
       <formula>LEN(TRIM(N2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O2:O14">
+  <conditionalFormatting sqref="O2:O18">
     <cfRule type="notContainsBlanks" dxfId="1" priority="11">
       <formula>LEN(TRIM(O2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R2:R13">
+  <conditionalFormatting sqref="R2:R17">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -1893,7 +2277,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2347,7 +2731,7 @@
         <v>1</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="4">
         <v>1</v>
@@ -2377,7 +2761,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -2386,10 +2770,10 @@
         <v>1</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -2411,28 +2795,204 @@
         <v>0</v>
       </c>
     </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="3">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" s="4">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14" s="4">
+        <v>1</v>
+      </c>
+      <c r="L14" s="3">
+        <f>IF(B14 = G14, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="3">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15" s="4">
+        <v>1</v>
+      </c>
+      <c r="L15" s="3">
+        <f>IF(B15 = G15, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="3">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16" s="4">
+        <v>1</v>
+      </c>
+      <c r="L16" s="3">
+        <f>IF(B16 = G16, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="3">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17" s="4">
+        <v>1</v>
+      </c>
+      <c r="L17" s="3">
+        <f>IF(B17 = G17, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D14">
+  <conditionalFormatting sqref="C2:C18">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="4">
+      <formula>LEN(TRIM(C2))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D18">
     <cfRule type="notContainsBlanks" dxfId="0" priority="2">
       <formula>LEN(TRIM(D2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E14">
+  <conditionalFormatting sqref="E2:E18">
     <cfRule type="notContainsBlanks" dxfId="0" priority="3">
       <formula>LEN(TRIM(E2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I14">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="4">
+  <conditionalFormatting sqref="F2:F18">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="5">
+      <formula>LEN(TRIM(F2))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H18">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="8">
+      <formula>LEN(TRIM(H2))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I18">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="6">
       <formula>LEN(TRIM(I2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J14">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="5">
+  <conditionalFormatting sqref="J2:J18">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="7">
       <formula>LEN(TRIM(J2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L13">
+  <conditionalFormatting sqref="K2:K18">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="9">
+      <formula>LEN(TRIM(K2))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L17">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -2448,7 +3008,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2457,10 +3017,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="11" width="12.28515625" customWidth="1"/>
+    <col min="1" max="15" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2473,26 +3033,38 @@
       <c r="D1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:14">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -2505,27 +3077,39 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2">
         <v>1</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="4">
         <v>1</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
-      <c r="I2" s="4">
-        <v>1</v>
-      </c>
-      <c r="J2" s="3">
-        <f>IF(B2 = F2, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" s="4">
+        <v>1</v>
+      </c>
+      <c r="N2" s="3">
+        <f>IF(B2 = H2, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -2538,27 +3122,39 @@
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3">
         <v>1</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="4">
         <v>1</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
-      <c r="I3" s="4">
-        <v>1</v>
-      </c>
-      <c r="J3" s="3">
-        <f>IF(B3 = F3, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3" s="4">
+        <v>1</v>
+      </c>
+      <c r="N3" s="3">
+        <f>IF(B3 = H3, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -2571,27 +3167,39 @@
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4">
         <v>1</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="4">
         <v>1</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
-      <c r="I4" s="4">
-        <v>1</v>
-      </c>
-      <c r="J4" s="3">
-        <f>IF(B4 = F4, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4" s="4">
+        <v>1</v>
+      </c>
+      <c r="N4" s="3">
+        <f>IF(B4 = H4, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -2604,27 +3212,39 @@
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="4">
         <v>1</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
-      <c r="I5" s="4">
-        <v>1</v>
-      </c>
-      <c r="J5" s="3">
-        <f>IF(B5 = F5, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5" s="4">
+        <v>1</v>
+      </c>
+      <c r="N5" s="3">
+        <f>IF(B5 = H5, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -2635,29 +3255,41 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6" s="4">
+        <v>1</v>
+      </c>
+      <c r="E6">
         <v>1</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="4">
         <v>1</v>
       </c>
       <c r="H6">
         <v>1</v>
       </c>
-      <c r="I6" s="4">
-        <v>1</v>
-      </c>
-      <c r="J6" s="3">
-        <f>IF(B6 = F6, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6" s="4">
+        <v>1</v>
+      </c>
+      <c r="N6" s="3">
+        <f>IF(B6 = H6, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -2668,29 +3300,41 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7">
         <v>1</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="4">
         <v>1</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
-      <c r="I7" s="4">
-        <v>1</v>
-      </c>
-      <c r="J7" s="3">
-        <f>IF(B7 = F7, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7" s="4">
+        <v>1</v>
+      </c>
+      <c r="N7" s="3">
+        <f>IF(B7 = H7, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -2701,29 +3345,41 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8">
         <v>1</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="4">
         <v>1</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
-      <c r="I8" s="4">
-        <v>1</v>
-      </c>
-      <c r="J8" s="3">
-        <f>IF(B8 = F8, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8" s="4">
+        <v>1</v>
+      </c>
+      <c r="N8" s="3">
+        <f>IF(B8 = H8, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -2734,29 +3390,41 @@
         <v>1</v>
       </c>
       <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9" s="4">
+        <v>1</v>
+      </c>
+      <c r="E9">
         <v>1</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="4">
         <v>1</v>
       </c>
       <c r="H9">
         <v>1</v>
       </c>
-      <c r="I9" s="4">
-        <v>1</v>
-      </c>
-      <c r="J9" s="3">
-        <f>IF(B9 = F9, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9" s="4">
+        <v>1</v>
+      </c>
+      <c r="N9" s="3">
+        <f>IF(B9 = H9, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -2767,29 +3435,41 @@
         <v>1</v>
       </c>
       <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10" s="4">
+        <v>1</v>
+      </c>
+      <c r="E10">
         <v>1</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="4">
         <v>1</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
-      <c r="I10" s="4">
-        <v>1</v>
-      </c>
-      <c r="J10" s="3">
-        <f>IF(B10 = F10, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10" s="4">
+        <v>1</v>
+      </c>
+      <c r="N10" s="3">
+        <f>IF(B10 = H10, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -2800,29 +3480,41 @@
         <v>1</v>
       </c>
       <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11" s="4">
+        <v>1</v>
+      </c>
+      <c r="E11">
         <v>1</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="4">
         <v>1</v>
       </c>
       <c r="H11">
         <v>1</v>
       </c>
-      <c r="I11" s="4">
-        <v>1</v>
-      </c>
-      <c r="J11" s="3">
-        <f>IF(B11 = F11, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11" s="4">
+        <v>1</v>
+      </c>
+      <c r="N11" s="3">
+        <f>IF(B11 = H11, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -2833,29 +3525,41 @@
         <v>1</v>
       </c>
       <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12" s="4">
+        <v>1</v>
+      </c>
+      <c r="E12">
         <v>1</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="4">
         <v>1</v>
       </c>
       <c r="H12">
         <v>1</v>
       </c>
-      <c r="I12" s="4">
-        <v>1</v>
-      </c>
-      <c r="J12" s="3">
-        <f>IF(B12 = F12, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12" s="4">
+        <v>1</v>
+      </c>
+      <c r="N12" s="3">
+        <f>IF(B12 = H12, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -2866,50 +3570,242 @@
         <v>1</v>
       </c>
       <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13" s="4">
+        <v>1</v>
+      </c>
+      <c r="E13">
         <v>1</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="4">
         <v>1</v>
       </c>
       <c r="H13">
         <v>1</v>
       </c>
-      <c r="I13" s="4">
-        <v>1</v>
-      </c>
-      <c r="J13" s="3">
-        <f>IF(B13 = F13, 1, 0)</f>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13" s="4">
+        <v>1</v>
+      </c>
+      <c r="N13" s="3">
+        <f>IF(B13 = H13, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="3">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" s="4">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14" s="4">
+        <v>1</v>
+      </c>
+      <c r="N14" s="3">
+        <f>IF(B14 = H14, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="3">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" s="4">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15" s="4">
+        <v>1</v>
+      </c>
+      <c r="N15" s="3">
+        <f>IF(B15 = H15, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="3">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" s="4">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16" s="4">
+        <v>1</v>
+      </c>
+      <c r="N16" s="3">
+        <f>IF(B16 = H16, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="3">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17" s="4">
+        <v>1</v>
+      </c>
+      <c r="N17" s="3">
+        <f>IF(B17 = H17, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C14">
+  <conditionalFormatting sqref="C2:C18">
     <cfRule type="notContainsBlanks" dxfId="0" priority="2">
       <formula>LEN(TRIM(C2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D14">
+  <conditionalFormatting sqref="D2:D18">
     <cfRule type="notContainsBlanks" dxfId="0" priority="3">
       <formula>LEN(TRIM(D2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G14">
+  <conditionalFormatting sqref="I2:I18">
     <cfRule type="notContainsBlanks" dxfId="0" priority="4">
-      <formula>LEN(TRIM(G2))&gt;0</formula>
+      <formula>LEN(TRIM(I2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H14">
+  <conditionalFormatting sqref="J2:J18">
     <cfRule type="notContainsBlanks" dxfId="0" priority="5">
-      <formula>LEN(TRIM(H2))&gt;0</formula>
+      <formula>LEN(TRIM(J2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J13">
+  <conditionalFormatting sqref="N2:N17">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -2925,7 +3821,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2934,10 +3830,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="9" width="12.28515625" customWidth="1"/>
+    <col min="1" max="15" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2947,23 +3843,41 @@
       <c r="C1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:14">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -2973,7 +3887,7 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
@@ -2985,12 +3899,30 @@
       <c r="G2" s="4">
         <v>1</v>
       </c>
-      <c r="H2" s="3">
-        <f>IF(B2 = E2, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" s="4">
+        <v>1</v>
+      </c>
+      <c r="N2" s="3">
+        <f>IF(B2 = H2, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -3000,7 +3932,7 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
@@ -3012,12 +3944,30 @@
       <c r="G3" s="4">
         <v>1</v>
       </c>
-      <c r="H3" s="3">
-        <f>IF(B3 = E3, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3" s="4">
+        <v>1</v>
+      </c>
+      <c r="N3" s="3">
+        <f>IF(B3 = H3, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -3027,7 +3977,7 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
@@ -3039,12 +3989,30 @@
       <c r="G4" s="4">
         <v>1</v>
       </c>
-      <c r="H4" s="3">
-        <f>IF(B4 = E4, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4" s="4">
+        <v>1</v>
+      </c>
+      <c r="N4" s="3">
+        <f>IF(B4 = H4, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -3054,7 +4022,7 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5">
         <v>1</v>
       </c>
       <c r="E5">
@@ -3066,12 +4034,30 @@
       <c r="G5" s="4">
         <v>1</v>
       </c>
-      <c r="H5" s="3">
-        <f>IF(B5 = E5, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5" s="4">
+        <v>1</v>
+      </c>
+      <c r="N5" s="3">
+        <f>IF(B5 = H5, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -3081,7 +4067,7 @@
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6">
         <v>1</v>
       </c>
       <c r="E6">
@@ -3093,12 +4079,30 @@
       <c r="G6" s="4">
         <v>1</v>
       </c>
-      <c r="H6" s="3">
-        <f>IF(B6 = E6, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6" s="4">
+        <v>1</v>
+      </c>
+      <c r="N6" s="3">
+        <f>IF(B6 = H6, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -3108,7 +4112,7 @@
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7">
         <v>1</v>
       </c>
       <c r="E7">
@@ -3120,12 +4124,30 @@
       <c r="G7" s="4">
         <v>1</v>
       </c>
-      <c r="H7" s="3">
-        <f>IF(B7 = E7, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7" s="4">
+        <v>1</v>
+      </c>
+      <c r="N7" s="3">
+        <f>IF(B7 = H7, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -3135,7 +4157,7 @@
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8">
         <v>1</v>
       </c>
       <c r="E8">
@@ -3147,12 +4169,30 @@
       <c r="G8" s="4">
         <v>1</v>
       </c>
-      <c r="H8" s="3">
-        <f>IF(B8 = E8, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8" s="4">
+        <v>1</v>
+      </c>
+      <c r="N8" s="3">
+        <f>IF(B8 = H8, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -3162,7 +4202,7 @@
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9">
         <v>1</v>
       </c>
       <c r="E9">
@@ -3174,12 +4214,30 @@
       <c r="G9" s="4">
         <v>1</v>
       </c>
-      <c r="H9" s="3">
-        <f>IF(B9 = E9, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9" s="4">
+        <v>1</v>
+      </c>
+      <c r="N9" s="3">
+        <f>IF(B9 = H9, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -3189,7 +4247,7 @@
       <c r="C10">
         <v>1</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10">
         <v>1</v>
       </c>
       <c r="E10">
@@ -3201,12 +4259,30 @@
       <c r="G10" s="4">
         <v>1</v>
       </c>
-      <c r="H10" s="3">
-        <f>IF(B10 = E10, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10" s="4">
+        <v>1</v>
+      </c>
+      <c r="N10" s="3">
+        <f>IF(B10 = H10, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -3216,7 +4292,7 @@
       <c r="C11">
         <v>1</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11">
         <v>1</v>
       </c>
       <c r="E11">
@@ -3228,12 +4304,30 @@
       <c r="G11" s="4">
         <v>1</v>
       </c>
-      <c r="H11" s="3">
-        <f>IF(B11 = E11, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11" s="4">
+        <v>1</v>
+      </c>
+      <c r="N11" s="3">
+        <f>IF(B11 = H11, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -3243,7 +4337,7 @@
       <c r="C12">
         <v>1</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12">
         <v>1</v>
       </c>
       <c r="E12">
@@ -3255,12 +4349,30 @@
       <c r="G12" s="4">
         <v>1</v>
       </c>
-      <c r="H12" s="3">
-        <f>IF(B12 = E12, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12" s="4">
+        <v>1</v>
+      </c>
+      <c r="N12" s="3">
+        <f>IF(B12 = H12, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -3270,7 +4382,7 @@
       <c r="C13">
         <v>1</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13">
         <v>1</v>
       </c>
       <c r="E13">
@@ -3282,13 +4394,211 @@
       <c r="G13" s="4">
         <v>1</v>
       </c>
-      <c r="H13" s="3">
-        <f>IF(B13 = E13, 1, 0)</f>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13" s="4">
+        <v>1</v>
+      </c>
+      <c r="N13" s="3">
+        <f>IF(B13 = H13, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="3">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14" s="4">
+        <v>1</v>
+      </c>
+      <c r="N14" s="3">
+        <f>IF(B14 = H14, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="3">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" s="4">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15" s="4">
+        <v>1</v>
+      </c>
+      <c r="N15" s="3">
+        <f>IF(B15 = H15, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="3">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" s="4">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16" s="4">
+        <v>1</v>
+      </c>
+      <c r="N16" s="3">
+        <f>IF(B16 = H16, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="3">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17" s="4">
+        <v>1</v>
+      </c>
+      <c r="N17" s="3">
+        <f>IF(B17 = H17, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H2:H13">
+  <conditionalFormatting sqref="N2:N17">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>

</xml_diff>